<commit_message>
updated reject and withdraw files
</commit_message>
<xml_diff>
--- a/IDs.xlsx
+++ b/IDs.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://tysononline-my.sharepoint.com/personal/harrison_heselbarth_tyson_com/Documents/Documents/Project Automation/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://tysononline-my.sharepoint.com/personal/harrison_heselbarth_tyson_com/Documents/Documents/Tyson-MRS-Tool/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="3" documentId="8_{4AB36AA9-3140-4406-8328-820C4BF913DE}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{271E8197-ECCC-4909-ADC0-B7A52CCB5D8D}"/>
+  <xr:revisionPtr revIDLastSave="7" documentId="8_{4AB36AA9-3140-4406-8328-820C4BF913DE}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{7D36EC8F-B39F-4EF6-B8C8-E592858B3440}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{C1103FB0-E295-4AC5-B361-5CB8053C089B}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{C1103FB0-E295-4AC5-B361-5CB8053C089B}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -380,62 +380,77 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B57AEDD0-DE11-4DC4-A7C1-95662CFFAFA5}">
-  <dimension ref="A1:A10"/>
+  <dimension ref="A1:A13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1">
-        <v>709911</v>
+        <v>710006</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>709914</v>
+        <v>710007</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3">
-        <v>709919</v>
+        <v>710014</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4">
-        <v>709923</v>
+        <v>710019</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5">
-        <v>709924</v>
+        <v>710034</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A6">
-        <v>709925</v>
+        <v>710077</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A7">
-        <v>709940</v>
+        <v>710083</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A8">
-        <v>709973</v>
+        <v>710084</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A9">
-        <v>709975</v>
+        <v>710003</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A10">
-        <v>710001</v>
+        <v>710000</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>710122</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>709877</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>711545</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fixed issue with 1 request doing more than 1
</commit_message>
<xml_diff>
--- a/IDs.xlsx
+++ b/IDs.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://tysononline-my.sharepoint.com/personal/harrison_heselbarth_tyson_com/Documents/Documents/Tyson-MRS-Tool/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="7" documentId="8_{4AB36AA9-3140-4406-8328-820C4BF913DE}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{7D36EC8F-B39F-4EF6-B8C8-E592858B3440}"/>
+  <xr:revisionPtr revIDLastSave="10" documentId="8_{4AB36AA9-3140-4406-8328-820C4BF913DE}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{B23684D9-DF8D-4D00-A5CA-362CFFAE91F1}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{C1103FB0-E295-4AC5-B361-5CB8053C089B}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{C1103FB0-E295-4AC5-B361-5CB8053C089B}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -380,77 +380,85 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B57AEDD0-DE11-4DC4-A7C1-95662CFFAFA5}">
-  <dimension ref="A1:A13"/>
+  <dimension ref="A1:A15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1">
-        <v>710006</v>
+        <v>699640</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>710007</v>
+        <v>699827</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3">
-        <v>710014</v>
+        <v>701350</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4">
-        <v>710019</v>
+        <v>701747</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5">
-        <v>710034</v>
+        <v>702499</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A6">
-        <v>710077</v>
+        <v>702850</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A7">
-        <v>710083</v>
+        <v>702951</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A8">
-        <v>710084</v>
+        <v>703205</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A9">
-        <v>710003</v>
+        <v>703347</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A10">
-        <v>710000</v>
+        <v>703400</v>
       </c>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A11">
-        <v>710122</v>
+        <v>703495</v>
       </c>
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A12">
-        <v>709877</v>
+        <v>703497</v>
       </c>
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A13">
-        <v>711545</v>
+        <v>703498</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>703740</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>703759</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fixing not going the full number of requests?
</commit_message>
<xml_diff>
--- a/IDs.xlsx
+++ b/IDs.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://tysononline-my.sharepoint.com/personal/harrison_heselbarth_tyson_com/Documents/Documents/Tyson-MRS-Tool/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="16" documentId="8_{4AB36AA9-3140-4406-8328-820C4BF913DE}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{EEDB8273-F41A-4BBE-B0BE-D0BA2CD44925}"/>
+  <xr:revisionPtr revIDLastSave="19" documentId="8_{4AB36AA9-3140-4406-8328-820C4BF913DE}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{0DB41EBA-6666-4EE1-BB9E-195237364C4E}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{C1103FB0-E295-4AC5-B361-5CB8053C089B}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{C1103FB0-E295-4AC5-B361-5CB8053C089B}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -380,22 +380,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B57AEDD0-DE11-4DC4-A7C1-95662CFFAFA5}">
-  <dimension ref="A1:A65"/>
+  <dimension ref="A1:A75"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:A65"/>
+    <sheetView tabSelected="1" topLeftCell="A49" workbookViewId="0">
+      <selection activeCell="B66" sqref="B66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1">
-        <v>699640</v>
+        <v>702850</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>699827</v>
+        <v>703400</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
@@ -405,312 +405,362 @@
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4">
-        <v>701747</v>
+        <v>703495</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5">
-        <v>702499</v>
+        <v>703497</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A6">
-        <v>702850</v>
+        <v>703498</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A7">
-        <v>702951</v>
+        <v>699640</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A8">
-        <v>703205</v>
+        <v>701747</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A9">
-        <v>703347</v>
+        <v>703740</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A10">
-        <v>703400</v>
+        <v>703873</v>
       </c>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A11">
-        <v>703495</v>
+        <v>703884</v>
       </c>
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A12">
-        <v>703497</v>
+        <v>703887</v>
       </c>
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A13">
-        <v>703498</v>
+        <v>703888</v>
       </c>
     </row>
     <row r="14" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A14">
-        <v>703740</v>
+        <v>703205</v>
       </c>
     </row>
     <row r="15" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A15">
-        <v>703759</v>
+        <v>703785</v>
       </c>
     </row>
     <row r="16" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A16">
-        <v>703781</v>
+        <v>703788</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A17">
-        <v>703785</v>
+        <v>703792</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A18">
-        <v>703788</v>
+        <v>703794</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A19">
-        <v>703792</v>
+        <v>703869</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A20">
-        <v>703794</v>
+        <v>703922</v>
       </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A21">
-        <v>703803</v>
+        <v>703929</v>
       </c>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A22">
-        <v>703869</v>
+        <v>703931</v>
       </c>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A23">
-        <v>703873</v>
+        <v>703935</v>
       </c>
     </row>
     <row r="24" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A24">
-        <v>703884</v>
+        <v>703937</v>
       </c>
     </row>
     <row r="25" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A25">
-        <v>703887</v>
+        <v>703347</v>
       </c>
     </row>
     <row r="26" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A26">
-        <v>703888</v>
+        <v>702951</v>
       </c>
     </row>
     <row r="27" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A27">
-        <v>703922</v>
+        <v>704031</v>
       </c>
     </row>
     <row r="28" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A28">
-        <v>703929</v>
+        <v>704036</v>
       </c>
     </row>
     <row r="29" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A29">
-        <v>703931</v>
+        <v>704049</v>
       </c>
     </row>
     <row r="30" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A30">
-        <v>703935</v>
+        <v>704028</v>
       </c>
     </row>
     <row r="31" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A31">
-        <v>703937</v>
+        <v>704029</v>
       </c>
     </row>
     <row r="32" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A32">
-        <v>704028</v>
+        <v>703759</v>
       </c>
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A33">
-        <v>704029</v>
+        <v>704061</v>
       </c>
     </row>
     <row r="34" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A34">
-        <v>704031</v>
+        <v>704063</v>
       </c>
     </row>
     <row r="35" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A35">
-        <v>704036</v>
+        <v>704067</v>
       </c>
     </row>
     <row r="36" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A36">
-        <v>704039</v>
+        <v>704069</v>
       </c>
     </row>
     <row r="37" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A37">
-        <v>704049</v>
+        <v>704077</v>
       </c>
     </row>
     <row r="38" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A38">
-        <v>704055</v>
+        <v>704120</v>
       </c>
     </row>
     <row r="39" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A39">
-        <v>704061</v>
+        <v>704121</v>
       </c>
     </row>
     <row r="40" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A40">
-        <v>704063</v>
+        <v>704127</v>
       </c>
     </row>
     <row r="41" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A41">
-        <v>704067</v>
+        <v>704133</v>
       </c>
     </row>
     <row r="42" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A42">
-        <v>704069</v>
+        <v>704143</v>
       </c>
     </row>
     <row r="43" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A43">
-        <v>704077</v>
+        <v>699827</v>
       </c>
     </row>
     <row r="44" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A44">
-        <v>704111</v>
+        <v>704219</v>
       </c>
     </row>
     <row r="45" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A45">
-        <v>704116</v>
+        <v>704222</v>
       </c>
     </row>
     <row r="46" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A46">
-        <v>704120</v>
+        <v>704226</v>
       </c>
     </row>
     <row r="47" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A47">
-        <v>704121</v>
+        <v>704239</v>
       </c>
     </row>
     <row r="48" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A48">
-        <v>704127</v>
+        <v>704241</v>
       </c>
     </row>
     <row r="49" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A49">
-        <v>704133</v>
+        <v>704248</v>
       </c>
     </row>
     <row r="50" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A50">
-        <v>704143</v>
+        <v>704235</v>
       </c>
     </row>
     <row r="51" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A51">
-        <v>704219</v>
+        <v>704237</v>
       </c>
     </row>
     <row r="52" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A52">
-        <v>704222</v>
+        <v>703803</v>
       </c>
     </row>
     <row r="53" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A53">
-        <v>704226</v>
+        <v>704259</v>
       </c>
     </row>
     <row r="54" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A54">
-        <v>704230</v>
+        <v>704116</v>
       </c>
     </row>
     <row r="55" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A55">
-        <v>704235</v>
+        <v>704055</v>
       </c>
     </row>
     <row r="56" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A56">
-        <v>704237</v>
+        <v>704324</v>
       </c>
     </row>
     <row r="57" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A57">
-        <v>704239</v>
+        <v>704418</v>
       </c>
     </row>
     <row r="58" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A58">
-        <v>704241</v>
+        <v>704607</v>
       </c>
     </row>
     <row r="59" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A59">
-        <v>704248</v>
+        <v>704608</v>
       </c>
     </row>
     <row r="60" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A60">
-        <v>704259</v>
+        <v>704613</v>
       </c>
     </row>
     <row r="61" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A61">
-        <v>704643</v>
+        <v>704630</v>
       </c>
     </row>
     <row r="62" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A62">
-        <v>704729</v>
+        <v>704666</v>
       </c>
     </row>
     <row r="63" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A63">
-        <v>704748</v>
+        <v>704672</v>
       </c>
     </row>
     <row r="64" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A64">
-        <v>704760</v>
+        <v>704681</v>
       </c>
     </row>
     <row r="65" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A65">
-        <v>704767</v>
+        <v>704696</v>
+      </c>
+    </row>
+    <row r="66" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A66">
+        <v>704803</v>
+      </c>
+    </row>
+    <row r="67" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A67">
+        <v>704805</v>
+      </c>
+    </row>
+    <row r="68" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A68">
+        <v>704870</v>
+      </c>
+    </row>
+    <row r="69" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A69">
+        <v>704928</v>
+      </c>
+    </row>
+    <row r="70" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A70">
+        <v>704929</v>
+      </c>
+    </row>
+    <row r="71" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A71">
+        <v>704941</v>
+      </c>
+    </row>
+    <row r="72" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A72">
+        <v>704947</v>
+      </c>
+    </row>
+    <row r="73" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A73">
+        <v>704949</v>
+      </c>
+    </row>
+    <row r="74" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A74">
+        <v>704960</v>
+      </c>
+    </row>
+    <row r="75" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A75">
+        <v>704976</v>
       </c>
     </row>
   </sheetData>

</xml_diff>